<commit_message>
new logic of iteration
</commit_message>
<xml_diff>
--- a/extracted_dates.xlsx
+++ b/extracted_dates.xlsx
@@ -4,7 +4,6 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet 2" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,336 +407,124 @@
         <v>Dated</v>
       </c>
       <c r="B1" t="str">
-        <v>Remarks</v>
-      </c>
-      <c r="C1" t="str">
-        <v>To</v>
-      </c>
-      <c r="D1" t="str">
         <v>GrandTotal</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B2" t="str">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B3" t="str">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B4" t="str">
+        <v>214</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B5" t="str">
+        <v>427</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B6" t="str">
+        <v>391</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B7" t="str">
+        <v>653</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B8" t="str">
+        <v>503</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B9" t="str">
+        <v>417</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B10" t="str">
+        <v>732</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B11" t="str">
+        <v>384</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B12" t="str">
+        <v>216</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B13" t="str">
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>19-10-2023</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B14" t="str">
+        <v>178</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>19-10-2023</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="str">
-        <v>QPSASPGEL202207</v>
-      </c>
-    </row>
-    <row r="30" xml:space="preserve">
-      <c r="C30" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="31" xml:space="preserve">
-      <c r="C31" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="32" xml:space="preserve">
-      <c r="C32" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="33" xml:space="preserve">
-      <c r="C33" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="34" xml:space="preserve">
-      <c r="C34" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="35" xml:space="preserve">
-      <c r="C35" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="36" xml:space="preserve">
-      <c r="C36" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="37" xml:space="preserve">
-      <c r="C37" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="38" xml:space="preserve">
-      <c r="C38" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="39" xml:space="preserve">
-      <c r="C39" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="40" xml:space="preserve">
-      <c r="C40" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="41" xml:space="preserve">
-      <c r="C41" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="42" xml:space="preserve">
-      <c r="C42" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="43" xml:space="preserve">
-      <c r="C43" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="44" xml:space="preserve">
-      <c r="C44" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-NAGARJUNA MEDICAL HALL[TL0039]</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="D45" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="D46" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="D47" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="D48" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="D49" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="D50" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="D51" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="D52" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="D53" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="D54" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="D55" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="D56" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="D57" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="D58" t="str">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="D59" t="str">
-        <v>18</v>
+        <v>Dated  :19-10-2023</v>
+      </c>
+      <c r="B15" t="str">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D59"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>